<commit_message>
added content to readme.md
</commit_message>
<xml_diff>
--- a/rejestr.xlsx
+++ b/rejestr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\projects\electrical_measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634A92A7-B158-4862-AC22-237BCAC0918B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7F41EE-1BD9-4E78-8DCA-0D259C052158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD12"/>
+      <selection activeCell="A2" sqref="A2:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>